<commit_message>
Adição dos Documentos de Gerencia
</commit_message>
<xml_diff>
--- a/doc/Garantia da Qualidade/ATR_Ata de Reunião.xlsx
+++ b/doc/Garantia da Qualidade/ATR_Ata de Reunião.xlsx
@@ -42,15 +42,6 @@
     <t>Problemas</t>
   </si>
   <si>
-    <t>Breno,Douglas, Graciano, Welder, Roger e Filipe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todos os membros da equipe concordaram em fazer suas respectivas atidades que estão no relatório de acompanhamento para </t>
-  </si>
-  <si>
-    <t>o dia 24/11.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Iniciar o Projeto Corruptos e Separação de Atividades                              </t>
   </si>
   <si>
@@ -58,6 +49,15 @@
   </si>
   <si>
     <t xml:space="preserve">                            Nomes                                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t>Todos os membros da equipe concordaram em fazer suas respectivas atidades que estão no Cronograma.</t>
+  </si>
+  <si>
+    <t>Breno,Douglas, Graciano, Welder, Roger, Rhawan e Filipe</t>
+  </si>
+  <si>
+    <t>Todos os membros concordaram de entregar suas tarefas na data estipulada.</t>
   </si>
 </sst>
 </file>
@@ -131,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -180,50 +180,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +602,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A24" sqref="A1:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,64 +612,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="126.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="13"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="5">
         <v>41237</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75">
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75">
+      <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75">
-      <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75">
-      <c r="A7" s="12" t="s">
+      <c r="B7" s="15"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.75">
-      <c r="A8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13"/>
+      <c r="B8" s="15"/>
     </row>
     <row r="9" spans="1:2" ht="15.75">
-      <c r="A9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="13"/>
+      <c r="A9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="7"/>
@@ -674,10 +688,10 @@
       <c r="B13" s="7"/>
     </row>
     <row r="14" spans="1:2" ht="15.75">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="16"/>
     </row>
     <row r="15" spans="1:2" ht="15.75">
       <c r="A15" s="7"/>
@@ -700,34 +714,34 @@
       <c r="B19" s="7"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6"/>
+      <c r="B20" s="10"/>
     </row>
     <row r="21" spans="1:2" ht="12" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:2" ht="15.75">
-      <c r="A22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" s="9"/>
+      <c r="A22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="11"/>
     </row>
     <row r="23" spans="1:2" ht="22.5">
-      <c r="A23" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="14"/>
+      <c r="A23" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:2" ht="15" customHeight="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1"/>
@@ -739,18 +753,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:B18"/>
@@ -759,6 +761,18 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>